<commit_message>
Inputable Cells for Observed Table; Adjust and Update Predictions
User now can either upload data or input observed daily data directly. Their input on day 0 and day 1 will update the predictions for the entire duration of the experiment.
</commit_message>
<xml_diff>
--- a/celldata.xlsx
+++ b/celldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khushi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\nakya-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D569D46A-EDB2-2441-909E-61B11DF59A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506CAA63-18D7-46F3-A0E4-88CA8FFB8409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{AB730A60-E070-DB4A-8BF2-9C96D52DA3F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB730A60-E070-DB4A-8BF2-9C96D52DA3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A241CF61-39A3-9748-AEF9-3E865694EBAC}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,107 +455,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>956949.1003628989</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1.5</v>
-      </c>
       <c r="B3">
-        <v>820110.43364600511</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>456949.10036289901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>820110.43364600511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>1723601.156960699</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2.5</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>2993657.5240874859</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>2828412.8733981312</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3.5</v>
-      </c>
-      <c r="B7">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>2984699.4576945822</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>3166443.706749748</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4.5</v>
-      </c>
-      <c r="B9">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>4113185.3448669091</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>4512520.3528595893</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>5.5</v>
-      </c>
-      <c r="B11">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>5355557.2857550187</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>5693093.0453154361</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>6.5</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>6475788.1657214472</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <v>6403050.0364428777</v>
       </c>
     </row>

</xml_diff>